<commit_message>
Backup folder - 2024-10-17 15:16:24
</commit_message>
<xml_diff>
--- a/Оптимізація та просування сайтів (SEO)/ЛР1/Розрахунки.xlsx
+++ b/Оптимізація та просування сайтів (SEO)/ЛР1/Розрахунки.xlsx
@@ -8,13 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yarik/Desktop/✈️ ХАІ 💻/Оптимізація та просування сайтів (SEO)/ЛР1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0227FD-BACB-8142-8E75-21D95F75BA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11498DA5-9FAD-2F4F-A7C9-C67E28129F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3980" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{6A60C6B0-5A9B-CF4B-9E9B-A42355DA15DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_Hlk144563280" localSheetId="0">Лист1!$A$28</definedName>
+    <definedName name="_Hlk144563371" localSheetId="0">Лист1!$A$30</definedName>
+    <definedName name="_Hlk144563397" localSheetId="0">Лист1!$A$31</definedName>
+    <definedName name="_Hlk144563559" localSheetId="0">Лист1!$A$34</definedName>
+    <definedName name="_Hlk144563581" localSheetId="0">Лист1!$A$35</definedName>
+    <definedName name="_xlchart.v5.0" hidden="1">Лист1!$A$14</definedName>
+    <definedName name="_xlchart.v5.1" hidden="1">Лист1!$A$15:$A$22</definedName>
+    <definedName name="_xlchart.v5.2" hidden="1">Лист1!$B$13:$B$14</definedName>
+    <definedName name="_xlchart.v5.3" hidden="1">Лист1!$B$15:$B$22</definedName>
+    <definedName name="_xlchart.v5.4" hidden="1">Лист1!$A$14</definedName>
+    <definedName name="_xlchart.v5.5" hidden="1">Лист1!$A$15:$A$22</definedName>
+    <definedName name="_xlchart.v5.6" hidden="1">Лист1!$B$13:$B$14</definedName>
+    <definedName name="_xlchart.v5.7" hidden="1">Лист1!$B$15:$B$22</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Aurora Trans</t>
   </si>
@@ -101,13 +116,40 @@
   </si>
   <si>
     <t>i</t>
+  </si>
+  <si>
+    <t>Параметр</t>
+  </si>
+  <si>
+    <t>Наявність електронної адреси, мобільного застосунку, посилань на розміщення в соціальних мережах</t>
+  </si>
+  <si>
+    <t>Тип конкуренції (прямий, непрямий, неявний)</t>
+  </si>
+  <si>
+    <t>Дизайн, навігація</t>
+  </si>
+  <si>
+    <t>Текстовий, фото, відео контент</t>
+  </si>
+  <si>
+    <t>Активність у соцмережах</t>
+  </si>
+  <si>
+    <t>Зворотній зв'язок з користувачем</t>
+  </si>
+  <si>
+    <t>Позиція в результатах пошуку</t>
+  </si>
+  <si>
+    <t>Цінова політика</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +185,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -158,12 +206,64 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -186,31 +286,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -228,6 +340,1114 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.27719901719901718"/>
+          <c:y val="0.20582909323066803"/>
+          <c:w val="0.44615862820587232"/>
+          <c:h val="0.74359771367645389"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Aurora Trans</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$A$28:$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Наявність електронної адреси, мобільного застосунку, посилань на розміщення в соціальних мережах</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Тип конкуренції (прямий, непрямий, неявний)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Дизайн, навігація</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Текстовий, фото, відео контент</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Активність у соцмережах</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Зворотній зв'язок з користувачем</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Позиція в результатах пошуку</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Цінова політика</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$28:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3DE1-CB40-9C7B-B385C2B63DDF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>АвтоТрансГарант</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$A$28:$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Наявність електронної адреси, мобільного застосунку, посилань на розміщення в соціальних мережах</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Тип конкуренції (прямий, непрямий, неявний)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Дизайн, навігація</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Текстовий, фото, відео контент</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Активність у соцмережах</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Зворотній зв'язок з користувачем</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Позиція в результатах пошуку</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Цінова політика</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$C$28:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3DE1-CB40-9C7B-B385C2B63DDF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Della</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Лист1!$A$28:$A$35</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Наявність електронної адреси, мобільного застосунку, посилань на розміщення в соціальних мережах</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Тип конкуренції (прямий, непрямий, неявний)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Дизайн, навігація</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Текстовий, фото, відео контент</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Активність у соцмережах</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Зворотній зв'язок з користувачем</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Позиція в результатах пошуку</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Цінова політика</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$28:$D$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3DE1-CB40-9C7B-B385C2B63DDF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="495452752"/>
+        <c:axId val="1234069599"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="495452752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1234069599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1234069599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-UA"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="495452752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-UA"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-UA"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1266190</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B90DBB-1BAC-642B-07F5-0212AD138EC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357BD5E5-1277-654B-B495-9BF21FD036F8}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,172 +1759,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>4</v>
       </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="6">
         <v>5</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>5</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="6">
         <v>5</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>5</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>4</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>5</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>4</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="6">
         <v>3</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="6">
         <v>5</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="6">
         <v>34</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <v>22</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="G13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
       <c r="F14" s="9" t="s">
         <v>13</v>
       </c>
@@ -721,30 +1941,30 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="7">
-        <f>B2/B2*100%</f>
-        <v>1</v>
-      </c>
-      <c r="C15" s="7">
+      <c r="B15" s="11">
+        <f>B2/C2*100%</f>
+        <v>4</v>
+      </c>
+      <c r="C15" s="11">
         <f>C2/$B2*100%</f>
         <v>0.25</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="11">
         <f>D2/$B2*100%</f>
         <v>0.25</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="3">
         <f>SUMPRODUCT($B$2:$B$9,$L$15:$L$22)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="3">
         <f>SUMPRODUCT($C$2:$C$9,$L$15:$L$22)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="3">
         <f>SUMPRODUCT($D$2:$D$9,$L$15:$L$22)</f>
         <v>0</v>
       </c>
@@ -756,18 +1976,18 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="7">
-        <f>B3/B3*100%</f>
-        <v>1</v>
-      </c>
-      <c r="C16" s="7">
+      <c r="B16" s="11">
+        <f t="shared" ref="B16:B22" si="0">B3/C3*100%</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="11">
         <f>C3/$B3*100%</f>
         <v>1</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="11">
         <f>D3/$B3*100%</f>
         <v>1</v>
       </c>
@@ -779,18 +1999,18 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="7">
-        <f>B4/B4*100%</f>
-        <v>1</v>
-      </c>
-      <c r="C17" s="7">
+      <c r="B17" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C17" s="11">
         <f>C4/$B4*100%</f>
         <v>0.2</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="11">
         <f>D4/$B4*100%</f>
         <v>0.4</v>
       </c>
@@ -802,18 +2022,18 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="7">
-        <f>B5/B5*100%</f>
-        <v>1</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="B18" s="11">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="C18" s="11">
         <f>C5/$B5*100%</f>
         <v>0.4</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="11">
         <f>D5/$B5*100%</f>
         <v>0.4</v>
       </c>
@@ -825,18 +2045,18 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="7">
-        <f>B6/B6*100%</f>
-        <v>1</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B19" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C19" s="11">
         <f>C6/$B6*100%</f>
         <v>1</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="11">
         <f>D6/$B6*100%</f>
         <v>1</v>
       </c>
@@ -848,18 +2068,18 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="7">
-        <f>B7/B7*100%</f>
-        <v>1</v>
-      </c>
-      <c r="C20" s="7">
+      <c r="B20" s="11">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="C20" s="11">
         <f>C7/$B7*100%</f>
         <v>0.8</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="11">
         <f>D7/$B7*100%</f>
         <v>0.2</v>
       </c>
@@ -871,18 +2091,18 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="7">
-        <f>B8/B8*100%</f>
-        <v>1</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="B21" s="11">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="C21" s="11">
         <f>C8/$B8*100%</f>
         <v>0.8</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="11">
         <f>D8/$B8*100%</f>
         <v>0.4</v>
       </c>
@@ -894,18 +2114,18 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="7">
-        <f>B9/B9*100%</f>
-        <v>1</v>
-      </c>
-      <c r="C22" s="7">
+      <c r="B22" s="11">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="C22" s="11">
         <f>C9/$B9*100%</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="11">
         <f>D9/$B9*100%</f>
         <v>0.66666666666666663</v>
       </c>
@@ -917,9 +2137,136 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="26" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:12" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="188" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="14">
+        <v>4</v>
+      </c>
+      <c r="C28" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="D28" s="14">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="14">
+        <v>1</v>
+      </c>
+      <c r="C29" s="14">
+        <v>1</v>
+      </c>
+      <c r="D29" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="14">
+        <v>5</v>
+      </c>
+      <c r="C30" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="D30" s="14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="14">
+        <v>2.5</v>
+      </c>
+      <c r="C31" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="D31" s="14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="14">
+        <v>1</v>
+      </c>
+      <c r="C32" s="14">
+        <v>1</v>
+      </c>
+      <c r="D32" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="C33" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D33" s="14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="C34" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D34" s="14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="C35" s="14">
+        <v>1.67</v>
+      </c>
+      <c r="D35" s="14">
+        <v>0.67</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -929,5 +2276,6 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>